<commit_message>
adding colors to site calendars
</commit_message>
<xml_diff>
--- a/Volunteer Schedules - Doodle.xlsx
+++ b/Volunteer Schedules - Doodle.xlsx
@@ -5702,7 +5702,6 @@
           <t>Anitra Freeman</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>12:30 PM
@@ -5715,7 +5714,6 @@
 4 h</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -5729,14 +5727,12 @@
 4 h</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>12:30 PM
 4 h</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -5756,8 +5752,6 @@
 4 h</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -5814,7 +5808,6 @@
 4 h</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5936,6 +5929,13 @@
 5 h</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -5943,6 +5943,7 @@
           <t>Ammanuel Haile-leul</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>9:30 AM
@@ -5992,6 +5993,8 @@
           <t>Anitra Freeman</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>2:00 PM
@@ -6004,6 +6007,8 @@
 4 h 30 min</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>2:00 PM
@@ -6023,12 +6028,19 @@
           <t>Anshul Tambay</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>9:30 AM
 5 h</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -6036,18 +6048,24 @@
           <t>Atthaya Chevaosot</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>2:00 PM
 3 h.1</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>2:00 PM
 3 h.1</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -6055,6 +6073,10 @@
           <t>Audrey Hoen</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>9:30 AM
@@ -6067,6 +6089,8 @@
 5 h</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -6074,6 +6098,8 @@
           <t>Cathea Carey</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>5:00 PM
@@ -6086,6 +6112,8 @@
 1 h 30 min</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>5:00 PM
@@ -6105,18 +6133,21 @@
           <t>Don Entner</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>9:30 AM
 5 h</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>1:30 PM
 5 h</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>9:30 AM
@@ -6129,6 +6160,7 @@
 5 h</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -6136,12 +6168,19 @@
           <t>Evan McLain</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>9:30 AM
 5 h</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -6210,12 +6249,18 @@
 3 h</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -6235,6 +6280,8 @@
 5 h</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>9:30 AM
@@ -6247,6 +6294,8 @@
 5 h</t>
         </is>
       </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -6266,6 +6315,12 @@
 4 h 30 min</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">

</xml_diff>

<commit_message>
updating schedule data from Doodle
</commit_message>
<xml_diff>
--- a/Volunteer Schedules - Doodle.xlsx
+++ b/Volunteer Schedules - Doodle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="19125" yWindow="45" windowWidth="19275" windowHeight="20835" tabRatio="600" firstSheet="7" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="19125" yWindow="45" windowWidth="19275" windowHeight="20835" tabRatio="600" firstSheet="4" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vashon Food Bank" sheetId="1" state="visible" r:id="rId1"/>
@@ -1555,7 +1555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1857,86 +1857,67 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Rumi Takahashi</t>
+          <t>Tracy Banaszynski</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:00 AM
+5 h</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>10:00 AM
+5 h</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11:00 AM
-3 h</t>
+          <t>10:00 AM
+5 h</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>10:00 AM
+5 h</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>11:00 AM
-3 h</t>
+          <t>10:00 AM
+5 h</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Tracy Banaszynski</t>
+          <t>Subregion</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10:00 AM
-5 h</t>
+          <t>North Seattle</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10:00 AM
-5 h</t>
+          <t>North Seattle</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10:00 AM
-5 h</t>
+          <t>North Seattle</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>10:00 AM
-5 h</t>
+          <t>North Seattle</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
-        <is>
-          <t>10:00 AM
-5 h</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Subregion</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>North Seattle</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>North Seattle</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>North Seattle</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>North Seattle</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
         <is>
           <t>North Seattle</t>
         </is>
@@ -2308,7 +2289,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2373,20 +2354,20 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Chris Pollina</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>10:00 AM
-3 h</t>
+          <t>Christopher Pollina</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10:00 AM
+5 h</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Christopher Pollina</t>
+          <t>Irwin Batara</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2396,6 +2377,12 @@
         </is>
       </c>
       <c r="D5" t="inlineStr">
+        <is>
+          <t>10:00 AM
+5 h</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>10:00 AM
 5 h</t>
@@ -2405,24 +2392,18 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Irwin Batara</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10:00 AM
-5 h</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>10:00 AM
-5 h</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10:00 AM
+          <t>Merylin Castelan</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12:00 PM
+5 h 30 min</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>12:00 PM
 5 h</t>
         </is>
       </c>
@@ -2430,26 +2411,26 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Merylin Castelan</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>12:00 PM
-5 h 30 min</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>12:00 PM
-5 h</t>
+          <t>Munira Girnary</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11:00 AM
+4 h</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>11:00 AM
+4 h</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Munira Girnary</t>
+          <t>Peggy Thesing</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2458,23 +2439,35 @@
 4 h</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>12:00 PM
+5 h</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>11:00 AM
+4 h</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>11:00 AM
 4 h</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>12:00 PM
+5 h</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Peggy Thesing</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>11:00 AM
-4 h</t>
+          <t>Ruby Wishnietsky</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2485,19 +2478,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>11:00 AM
-4 h</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>11:00 AM
-4 h</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>12:00 PM
+          <t>10:00 AM
 5 h</t>
         </is>
       </c>
@@ -2505,49 +2486,30 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ruby Wishnietsky</t>
+          <t>Subregion</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>North King County</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12:00 PM
-5 h</t>
+          <t>North King County</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10:00 AM
-5 h</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Subregion</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
           <t>North King County</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>North King County</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>North King County</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>North King County</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>North King County</t>
         </is>
@@ -3166,7 +3128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3269,10 +3231,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B Pepowski</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+          <t>Brett Pepowski</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5:00 PM
+3 h</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5:00 PM
+3 h</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>5:00 PM
 3 h</t>
@@ -3282,24 +3256,42 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Brett Pepowski</t>
+          <t>Catherine Todd</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>5:00 PM
-3 h</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>5:00 PM
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>5:00 PM
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
@@ -3307,42 +3299,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Catherine Todd</t>
+          <t>Daniela Maqueda</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2:00 PM
+3 h</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>8:00 AM
+          <t>2:00 PM
 3 h</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>8:00 AM
+          <t>2:00 PM
 3 h</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>8:00 AM
+          <t>2:00 PM
 3 h</t>
         </is>
       </c>
@@ -3350,30 +3330,18 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Daniela Maqueda</t>
+          <t>Grace Lee</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2:00 PM
-3 h</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2:00 PM
-3 h</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2:00 PM
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2:00 PM
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
@@ -3381,18 +3349,42 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Grace Lee</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5:00 PM
+          <t>Hope Ambachew</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5:00 PM
+          <t>2:00 PM
+3 h</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
@@ -3400,42 +3392,30 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hope Ambachew</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>8:00 AM
+          <t>Irene Hsiao</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00 AM
 3 h</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2:00 PM
-3 h</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>8:00 AM
+          <t>11:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>11:00 AM
 3 h</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>8:00 AM
+          <t>11:00 AM
 3 h</t>
         </is>
       </c>
@@ -3443,22 +3423,10 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Irene Hsiao</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>11:00 AM
-3 h</t>
+          <t>Jenna Dee</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
-        <is>
-          <t>11:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
@@ -3474,16 +3442,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Jenna Dee</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>11:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
+          <t>Jocelyn Le</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
@@ -3493,16 +3461,52 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jocelyn Le</t>
+          <t>Maria Covert</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2:00 PM
+3 h</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2:00 PM
+3 h</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>11:00 AM
 3 h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
@@ -3512,54 +3516,54 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Maria Covert</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>8:00 AM
-3 h</t>
+          <t>Miriam Albdairi</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2:00 PM
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2:00 PM
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>11:00 AM
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>8:00 AM
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>8:00 AM
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>8:00 AM
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>11:00 AM
+          <t>5:00 PM
+3 h</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>5:00 PM
 3 h</t>
         </is>
       </c>
@@ -3567,54 +3571,48 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Miriam Albdairi</t>
+          <t>Ruby Tuesday Romero</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11:00 AM
+3 h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5:00 PM
+          <t>11:00 AM
 3 h</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5:00 PM
-3 h</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>5:00 PM
+          <t>11:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>11:00 AM
 3 h</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5:00 PM
-3 h</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>5:00 PM
-3 h</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>5:00 PM
+          <t>11:00 AM
 3 h</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>5:00 PM
+          <t>11:00 AM
 3 h</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>5:00 PM
+          <t>11:00 AM
 3 h</t>
         </is>
       </c>
@@ -3622,48 +3620,54 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ruby Tuesday Romero</t>
+          <t>Shaurya Addagatla</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11:00 AM
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11:00 AM
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11:00 AM
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>11:00 AM
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>11:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>11:00 AM
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>8:00 AM
+3 h</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>11:00 AM
+          <t>8:00 AM
 3 h</t>
         </is>
       </c>
@@ -3671,54 +3675,18 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Shaurya Addagatla</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>8:00 AM
-3 h</t>
+          <t>Vishya Adipudi</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>8:00 AM
+          <t>2:00 PM
 3 h</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>8:00 AM
-3 h</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>8:00 AM
+          <t>2:00 PM
 3 h</t>
         </is>
       </c>
@@ -3726,74 +3694,55 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Vishya Adipudi</t>
+          <t>Subregion</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Family Phone Line</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Family Phone Line</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Family Phone Line</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Family Phone Line</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Family Phone Line</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2:00 PM
-3 h</t>
+          <t>Family Phone Line</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Family Phone Line</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2:00 PM
-3 h</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Subregion</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
           <t>Family Phone Line</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Family Phone Line</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Family Phone Line</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Family Phone Line</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Family Phone Line</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Family Phone Line</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Family Phone Line</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Family Phone Line</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Family Phone Line</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>Family Phone Line</t>
         </is>
@@ -5421,6 +5370,7 @@
           <t>Ann Vander Stoep</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>11:00 AM
@@ -5439,12 +5389,16 @@
 3 h</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>11:00 AM
@@ -5458,6 +5412,14 @@
           <t>Ellen Waters</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
           <t>11:00 AM
@@ -5477,6 +5439,9 @@
           <t>Gail Emanuel</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>11:00 AM
@@ -5495,6 +5460,8 @@
 3 h</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
           <t>11:00 AM
@@ -5520,12 +5487,14 @@
 3 h.1</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h.1</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>11:00 AM
@@ -5538,6 +5507,10 @@
 3 h</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5545,30 +5518,36 @@
           <t>Mahika Bagri</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5576,6 +5555,9 @@
           <t>Maria Lynn Arns</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>11:00 AM
@@ -5588,6 +5570,9 @@
 3 h</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
           <t>11:00 AM
@@ -5929,13 +5914,6 @@
 5 h</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -5943,7 +5921,6 @@
           <t>Ammanuel Haile-leul</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>9:30 AM
@@ -5993,8 +5970,6 @@
           <t>Anitra Freeman</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>2:00 PM
@@ -6007,8 +5982,6 @@
 4 h 30 min</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>2:00 PM
@@ -6028,19 +6001,12 @@
           <t>Anshul Tambay</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>9:30 AM
 5 h</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -6048,24 +6014,18 @@
           <t>Atthaya Chevaosot</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>2:00 PM
 3 h.1</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>2:00 PM
 3 h.1</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -6073,10 +6033,6 @@
           <t>Audrey Hoen</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>9:30 AM
@@ -6089,8 +6045,6 @@
 5 h</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -6098,8 +6052,6 @@
           <t>Cathea Carey</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>5:00 PM
@@ -6112,8 +6064,6 @@
 1 h 30 min</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>5:00 PM
@@ -6133,21 +6083,18 @@
           <t>Don Entner</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>9:30 AM
 5 h</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>1:30 PM
 5 h</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>9:30 AM
@@ -6160,7 +6107,6 @@
 5 h</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -6168,19 +6114,12 @@
           <t>Evan McLain</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>9:30 AM
 5 h</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -6249,18 +6188,12 @@
 3 h</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
           <t>11:00 AM
 3 h</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -6280,8 +6213,6 @@
 5 h</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>9:30 AM
@@ -6294,8 +6225,6 @@
 5 h</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -6315,12 +6244,6 @@
 4 h 30 min</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">

</xml_diff>

<commit_message>
added map links to one-pagers
</commit_message>
<xml_diff>
--- a/Volunteer Schedules - Doodle.xlsx
+++ b/Volunteer Schedules - Doodle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kcrhaorg-my.sharepoint.com/personal/ben_mathewson_kcrha_org/Documents/GitHub/KCRHA-PIT-Count.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_08223C602990A987F5E5BE90394B40E970BB97C3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE85722F-0C46-4C1C-ACD6-764232A85464}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_0403FC412926AFFF4877A1A9B92B04F5B69BE214" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8AB2C71-5F41-430C-94C1-C132BD1ED7BC}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="75" windowWidth="19335" windowHeight="20835" firstSheet="23" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19155" yWindow="75" windowWidth="19275" windowHeight="20835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vashon Island Library" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="218">
   <si>
     <t>Name</t>
   </si>
@@ -103,11 +103,14 @@
 3 h 30 min</t>
   </si>
   <si>
-    <t>Caroline Herre</t>
+    <t>Brandon Morande</t>
   </si>
   <si>
     <t>10:30 AM
 4 h</t>
+  </si>
+  <si>
+    <t>Caroline Herre</t>
   </si>
   <si>
     <t>Charles Williams</t>
@@ -1099,15 +1102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1222,16 +1219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1255,140 +1245,140 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
         <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
         <v>73</v>
-      </c>
-      <c r="F6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
         <v>73</v>
-      </c>
-      <c r="F7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
         <v>73</v>
-      </c>
-      <c r="F9" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
         <v>73</v>
-      </c>
-      <c r="F10" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1396,19 +1386,19 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1420,15 +1410,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1455,68 +1439,68 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" t="s">
-        <v>85</v>
-      </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1524,22 +1508,22 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1551,15 +1535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1586,56 +1564,56 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1643,22 +1621,22 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1670,15 +1648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1702,39 +1674,39 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1742,19 +1714,19 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1766,15 +1738,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1810,89 +1776,89 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
         <v>95</v>
       </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1900,31 +1866,31 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1936,15 +1902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1968,29 +1928,29 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -2004,137 +1964,137 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2142,19 +2102,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2166,15 +2126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2198,135 +2152,135 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -2340,19 +2294,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2360,19 +2314,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2384,16 +2338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2417,7 +2364,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -2425,51 +2372,51 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -2480,13 +2427,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D8" t="s">
         <v>2</v>
@@ -2495,18 +2442,18 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2514,19 +2461,19 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2538,15 +2485,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2570,92 +2511,92 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2663,202 +2604,202 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2866,19 +2807,19 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2890,15 +2831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2937,282 +2872,282 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" t="s">
         <v>148</v>
       </c>
-      <c r="F3" t="s">
-        <v>147</v>
-      </c>
       <c r="G3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3220,34 +3155,34 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3259,15 +3194,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3318,15 +3247,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3350,112 +3273,112 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
         <v>169</v>
       </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>168</v>
-      </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3463,19 +3386,19 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3487,17 +3410,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3521,16 +3436,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -3541,27 +3456,27 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -3572,13 +3487,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3586,19 +3501,19 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3610,15 +3525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3642,84 +3551,84 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3727,19 +3636,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3751,15 +3660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3783,130 +3686,130 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3914,19 +3817,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3938,16 +3841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3968,83 +3864,83 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" t="s">
         <v>192</v>
       </c>
-      <c r="B6" t="s">
-        <v>191</v>
-      </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4052,16 +3948,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4073,15 +3969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -4114,53 +4004,53 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -4168,29 +4058,29 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4198,109 +4088,109 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4308,28 +4198,28 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4341,15 +4231,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -4373,66 +4259,66 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -4443,61 +4329,61 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -4511,7 +4397,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -4525,7 +4411,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -4539,16 +4425,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4556,19 +4442,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4580,15 +4466,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -4627,104 +4507,104 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -4732,34 +4612,34 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4769,15 +4649,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
@@ -4824,7 +4704,7 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4832,51 +4712,48 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
+      <c r="F4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4884,14 +4761,11 @@
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
+      <c r="B9" t="s">
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4901,26 +4775,29 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4928,22 +4805,10 @@
       <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
       <c r="F13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4983,28 +4848,51 @@
       <c r="D15" t="s">
         <v>18</v>
       </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" t="s">
-        <v>31</v>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -5016,15 +4904,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5048,58 +4930,58 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5107,19 +4989,19 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -5131,15 +5013,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5160,74 +5036,74 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
@@ -5235,10 +5111,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -5246,16 +5122,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -5267,15 +5143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5299,10 +5169,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -5313,42 +5183,42 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5356,19 +5226,19 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -5380,15 +5250,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5412,81 +5276,81 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5494,19 +5358,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -5518,15 +5382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5547,64 +5405,64 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5612,16 +5470,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -5633,14 +5491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5664,35 +5517,35 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -5712,46 +5565,46 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -5774,19 +5627,19 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>